<commit_message>
Added time validation to TextBox.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-revised.xlsx
+++ b/docs/dev-plan-revised.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\accenture-mdh\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace-web\mdh\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="18732" windowHeight="8100"/>
+    <workbookView xWindow="3735" yWindow="0" windowWidth="18735" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$75</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -782,18 +782,18 @@
       <selection activeCell="E2" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="53.109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" style="11" customWidth="1"/>
     <col min="6" max="6" width="24" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="11"/>
+    <col min="7" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -813,7 +813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>42899</v>
       </c>
@@ -829,7 +829,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>42900</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="D3" s="19"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>42901</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>42902</v>
       </c>
@@ -871,7 +871,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>42905</v>
       </c>
@@ -885,7 +885,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>42906</v>
       </c>
@@ -899,7 +899,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>42907</v>
       </c>
@@ -913,7 +913,7 @@
       <c r="D8" s="19"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>42908</v>
       </c>
@@ -927,7 +927,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>42909</v>
       </c>
@@ -941,7 +941,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="22"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>42912</v>
       </c>
@@ -954,7 +954,7 @@
       </c>
       <c r="E11" s="22"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>42913</v>
       </c>
@@ -967,7 +967,7 @@
       </c>
       <c r="E12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>42914</v>
       </c>
@@ -980,7 +980,7 @@
       </c>
       <c r="E13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>42915</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>42916</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>42919</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>42920</v>
       </c>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>42921</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E18" s="22"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>42922</v>
       </c>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>42923</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="E20" s="22"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>42926</v>
       </c>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="E21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>42927</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="E22" s="22"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>42928</v>
       </c>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>42929</v>
       </c>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>42930</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>42933</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>42934</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>42935</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>42936</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>42937</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>42940</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>42941</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>42942</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>42943</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>42944</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>42947</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>42948</v>
       </c>
@@ -1312,7 +1312,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>42949</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>42950</v>
       </c>
@@ -1340,7 +1340,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>42951</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>42954</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>42955</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>42956</v>
       </c>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>42957</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>42958</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>42961</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>42962</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>42963</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <v>42964</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>42965</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>42968</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <v>42969</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <v>42970</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>42971</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>42972</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>42975</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
         <v>42976</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
         <v>42977</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
         <v>42978</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>42979</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
         <v>42982</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
         <v>42983</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
         <v>42984</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
         <v>42985</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>42986</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>42989</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
         <v>42990</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
         <v>42991</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
         <v>42992</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
         <v>42993</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
         <v>42996</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
         <v>42997</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
         <v>42998</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
         <v>42999</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
         <v>43000</v>
       </c>

</xml_diff>